<commit_message>
anh nao sua phan cua toi day
</commit_message>
<xml_diff>
--- a/src/public/exports/PhuLucGiangVienMoi.xlsx
+++ b/src/public/exports/PhuLucGiangVienMoi.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="32">
   <si>
     <t>Ban Cơ yếu Chính phủ</t>
   </si>
@@ -214,16 +214,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,9 +565,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -756,12 +753,8 @@
       <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="11">
         <v>65</v>
       </c>
@@ -791,15 +784,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -807,9 +800,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -1036,12 +1026,8 @@
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="11">
         <v>200</v>
       </c>
@@ -1071,15 +1057,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -1087,9 +1073,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -1316,12 +1299,8 @@
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="11">
         <v>216</v>
       </c>
@@ -1351,15 +1330,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix duyệt đào tạo, tài hcính (info2), đổi lại cách lưu và xuất hợp đồng cho phù hợp với ngày bắt đầu min và ngày kết thúc max
</commit_message>
<xml_diff>
--- a/src/public/exports/PhuLucGiangVienMoi.xlsx
+++ b/src/public/exports/PhuLucGiangVienMoi.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="40">
   <si>
     <t>Ban Cơ yếu Chính phủ</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Đoàn Minh Phương</t>
+  </si>
+  <si>
+    <t>A18-Kỹ nghệ ATM01</t>
+  </si>
+  <si>
+    <t>An toàn mạng không dây và di động</t>
+  </si>
+  <si>
+    <t>11/1/2024 - 11/3/2024</t>
+  </si>
+  <si>
+    <t>Khai thác lỗ hổng phần mềm</t>
   </si>
   <si>
     <t>A20C8D701</t>
@@ -584,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
@@ -776,13 +788,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" s="10">
         <v>110</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="11">
         <v>1</v>
@@ -806,38 +818,342 @@
         <v>9900000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10">
+        <v>110</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="10">
+        <v>4</v>
+      </c>
+      <c r="I10" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L10" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="10">
+        <v>110</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="10">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L11" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="10">
+        <v>110</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L12" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="10">
+        <v>110</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10">
+        <v>4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L13" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10">
+        <v>110</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="10">
+        <v>4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L14" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="10">
+        <v>110</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="10">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L15" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10">
+        <v>110</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="10">
+        <v>4</v>
+      </c>
+      <c r="I16" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L16" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="10">
+        <v>110</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="10">
+        <v>4</v>
+      </c>
+      <c r="I17" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="L17" s="8">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12">
-        <v>220</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="12">
-        <v>22000000</v>
-      </c>
-      <c r="K10" s="12">
-        <v>2200000</v>
-      </c>
-      <c r="L10" s="12">
-        <v>19800000</v>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12">
+        <v>1100</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="12">
+        <v>110000000</v>
+      </c>
+      <c r="K18" s="12">
+        <v>11000000</v>
+      </c>
+      <c r="L18" s="12">
+        <v>99000000</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +1164,7 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -857,7 +1173,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
@@ -1049,7 +1365,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10">
         <v>100</v>
@@ -1079,38 +1395,342 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="10">
+        <v>4</v>
+      </c>
+      <c r="I10" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L10" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="10">
+        <v>100</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="10">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L11" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10">
+        <v>100</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L12" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="10">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10">
+        <v>4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L13" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10">
+        <v>100</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="10">
+        <v>4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L14" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="10">
+        <v>100</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="10">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L15" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="10">
+        <v>100</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="10">
+        <v>4</v>
+      </c>
+      <c r="I16" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L16" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="10">
+        <v>100</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="10">
+        <v>4</v>
+      </c>
+      <c r="I17" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="L17" s="8">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12">
-        <v>200</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="12">
-        <v>20000000</v>
-      </c>
-      <c r="K10" s="12">
-        <v>2000000</v>
-      </c>
-      <c r="L10" s="12">
-        <v>18000000</v>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="12">
+        <v>100000000</v>
+      </c>
+      <c r="K18" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="L18" s="12">
+        <v>90000000</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1741,7 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -1130,7 +1750,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L42"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
@@ -1287,7 +1907,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="10">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>32</v>
@@ -1296,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H8" s="10">
         <v>4</v>
@@ -1305,13 +1925,13 @@
         <v>100000</v>
       </c>
       <c r="J8" s="8">
-        <v>17300000</v>
+        <v>14100000</v>
       </c>
       <c r="K8" s="8">
-        <v>1730000</v>
+        <v>1410000</v>
       </c>
       <c r="L8" s="8">
-        <v>15570000</v>
+        <v>12690000</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1322,7 +1942,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="10">
         <v>173</v>
@@ -1334,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H9" s="10">
         <v>4</v>
@@ -1360,19 +1980,19 @@
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="10">
         <v>173</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="11">
         <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H10" s="10">
         <v>4</v>
@@ -1390,38 +2010,1216 @@
         <v>15570000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="10">
+        <v>141</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="10">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L11" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="10">
+        <v>173</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L12" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="10">
+        <v>173</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="10">
+        <v>4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L13" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="10">
+        <v>173</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="10">
+        <v>4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L14" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="10">
+        <v>141</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="10">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L15" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="10">
+        <v>173</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="10">
+        <v>4</v>
+      </c>
+      <c r="I16" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L16" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="10">
+        <v>141</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="10">
+        <v>4</v>
+      </c>
+      <c r="I17" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L17" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="10">
+        <v>173</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="10">
+        <v>4</v>
+      </c>
+      <c r="I18" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J18" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L18" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="10">
+        <v>141</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="10">
+        <v>4</v>
+      </c>
+      <c r="I19" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J19" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L19" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="10">
+        <v>141</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="10">
+        <v>4</v>
+      </c>
+      <c r="I20" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J20" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K20" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L20" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="10">
+        <v>141</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="10">
+        <v>4</v>
+      </c>
+      <c r="I21" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J21" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L21" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="10">
+        <v>173</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="10">
+        <v>4</v>
+      </c>
+      <c r="I22" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J22" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K22" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L22" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="10">
+        <v>141</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="11">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="10">
+        <v>4</v>
+      </c>
+      <c r="I23" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J23" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K23" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L23" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="10">
+        <v>173</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="11">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="10">
+        <v>4</v>
+      </c>
+      <c r="I24" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J24" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L24" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="10">
+        <v>141</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="10">
+        <v>4</v>
+      </c>
+      <c r="I25" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J25" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L25" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="10">
+        <v>173</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="11">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="10">
+        <v>4</v>
+      </c>
+      <c r="I26" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J26" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K26" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L26" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="10">
+        <v>141</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="11">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="10">
+        <v>4</v>
+      </c>
+      <c r="I27" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J27" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K27" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L27" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="10">
+        <v>141</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="10">
+        <v>4</v>
+      </c>
+      <c r="I28" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J28" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K28" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L28" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="10">
+        <v>141</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="10">
+        <v>4</v>
+      </c>
+      <c r="I29" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J29" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L29" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="10">
+        <v>173</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="11">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="10">
+        <v>4</v>
+      </c>
+      <c r="I30" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J30" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L30" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="10">
+        <v>173</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="10">
+        <v>4</v>
+      </c>
+      <c r="I31" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J31" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L31" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="10">
+        <v>141</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="11">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="10">
+        <v>4</v>
+      </c>
+      <c r="I32" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J32" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K32" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L32" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="10">
+        <v>141</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="11">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="10">
+        <v>4</v>
+      </c>
+      <c r="I33" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J33" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K33" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L33" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="10">
+        <v>173</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="11">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="10">
+        <v>4</v>
+      </c>
+      <c r="I34" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J34" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L34" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="10">
+        <v>173</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="10">
+        <v>4</v>
+      </c>
+      <c r="I35" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J35" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K35" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L35" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="10">
+        <v>173</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="11">
+        <v>1</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="10">
+        <v>4</v>
+      </c>
+      <c r="I36" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J36" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K36" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L36" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="10">
+        <v>141</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="11">
+        <v>1</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="10">
+        <v>4</v>
+      </c>
+      <c r="I37" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J37" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K37" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L37" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="10">
+        <v>173</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="11">
+        <v>1</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="10">
+        <v>4</v>
+      </c>
+      <c r="I38" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J38" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K38" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L38" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="10">
+        <v>141</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="11">
+        <v>1</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="10">
+        <v>4</v>
+      </c>
+      <c r="I39" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J39" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K39" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L39" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="10">
+        <v>173</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="11">
+        <v>1</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="10">
+        <v>4</v>
+      </c>
+      <c r="I40" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J40" s="8">
+        <v>17300000</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1730000</v>
+      </c>
+      <c r="L40" s="8">
+        <v>15570000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="10">
+        <v>141</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="11">
+        <v>1</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="10">
+        <v>4</v>
+      </c>
+      <c r="I41" s="8">
+        <v>100000</v>
+      </c>
+      <c r="J41" s="8">
+        <v>14100000</v>
+      </c>
+      <c r="K41" s="8">
+        <v>1410000</v>
+      </c>
+      <c r="L41" s="8">
+        <v>12690000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12">
-        <v>519</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="12">
-        <v>51900000</v>
-      </c>
-      <c r="K11" s="12">
-        <v>5190000</v>
-      </c>
-      <c r="L11" s="12">
-        <v>46710000</v>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12">
+        <v>5338</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="12">
+        <v>533800000</v>
+      </c>
+      <c r="K42" s="12">
+        <v>53380000</v>
+      </c>
+      <c r="L42" s="12">
+        <v>480420000</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +3230,7 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A42:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>